<commit_message>
Add test case an edit Tambah Pelanggan, Edit Pelanggan, Cek Pelanggan, Tambah Alamat, Edit Alamat, Hapus Alamat, Top Up Pelanggan, Hapus Pelanggan. Add test data terkait Pelanggan dan Pelanggan_edit
</commit_message>
<xml_diff>
--- a/Excel/PelangganDataExcel.xlsx
+++ b/Excel/PelangganDataExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>namapelanggan</t>
   </si>
@@ -77,6 +77,9 @@
     <t>emailpj</t>
   </si>
   <si>
+    <t>topup</t>
+  </si>
+  <si>
     <t>Sunari Ngatmono</t>
   </si>
   <si>
@@ -123,6 +126,9 @@
   </si>
   <si>
     <t>pjsunari@mail.com</t>
+  </si>
+  <si>
+    <t>10000</t>
   </si>
 </sst>
 </file>
@@ -1284,10 +1290,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1306,7 +1312,7 @@
     <col min="16" max="16" width="18.7272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1355,55 +1361,61 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:16">
+    <row r="2" s="1" customFormat="1" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>